<commit_message>
updates to metadata, moved Dendra download
</commit_message>
<xml_diff>
--- a/data/station_instrumentation/climate/climate_metadata.xlsx
+++ b/data/station_instrumentation/climate/climate_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zanedamico/UC Berkeley/Meadows/sagehen_meadows/data/climate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnat/Documents/GitHub/sagehen_meadows/data/station_instrumentation/climate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225B51CB-F656-6548-9AC9-D550248DFF88}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C72650B-AF1E-D44D-9C4B-A59C33944994}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="460" windowWidth="32780" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - climate_metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
   <si>
     <t>Source</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Relative Humidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snow Water Equivalent (SWE), </t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +233,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -295,7 +304,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -329,9 +338,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -343,6 +349,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1505,10 +1517,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="75" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>
@@ -1516,11 +1528,11 @@
     <col min="1" max="1" width="81" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="50.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" style="1" bestFit="1" customWidth="1"/>
@@ -1529,17 +1541,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
     </row>
     <row r="2" spans="1:11" ht="25">
       <c r="A2" s="2" t="s">
@@ -1716,10 +1728,10 @@
       <c r="E7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="15">
         <v>43009</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="15">
         <v>43770</v>
       </c>
       <c r="H7" s="5" t="s">
@@ -1747,10 +1759,10 @@
       <c r="E8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="15">
         <v>43009</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="15">
         <v>43770</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -1883,35 +1895,18 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="25">
-      <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="5">
-        <v>2151773.3686099998</v>
-      </c>
-      <c r="C13" s="5">
-        <v>697491.42197100003</v>
-      </c>
-      <c r="D13" s="9">
-        <v>1931.5175999999999</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>45</v>
+      <c r="A13" s="3"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="9"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="16" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="104">
+    <row r="14" spans="1:11" ht="25">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -1924,8 +1919,8 @@
       <c r="D14" s="9">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>35</v>
+      <c r="E14" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>26</v>
@@ -1937,86 +1932,115 @@
         <v>29</v>
       </c>
       <c r="I14" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="104">
+      <c r="A15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2151773.3686099998</v>
+      </c>
+      <c r="C15" s="5">
+        <v>697491.42197100003</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1931.5175999999999</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" ht="208">
-      <c r="A15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="8">
-        <v>38626</v>
-      </c>
-      <c r="G15" s="8">
-        <v>39721.979166666664</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>42</v>
-      </c>
+      <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="25">
-      <c r="A16" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="5"/>
+    <row r="16" spans="1:11" ht="208">
+      <c r="A16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>43</v>
+      <c r="F16" s="8">
+        <v>38626</v>
+      </c>
+      <c r="G16" s="8">
+        <v>39721.979166666664</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" ht="25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="7"/>
+      <c r="I17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" ht="25">
-      <c r="I18" s="7"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" ht="25">
-      <c r="A19" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:11" ht="20" customHeight="1">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:11" ht="25">
+      <c r="A20" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" ht="20" customHeight="1">
+      <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I20" s="7"/>
+      <c r="I21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2027,8 +2051,8 @@
     <hyperlink ref="A5" r:id="rId2" display="Hobo Logger #496" xr:uid="{2C62D66F-6380-E646-8CDF-4F5015D49CEF}"/>
     <hyperlink ref="A4" r:id="rId3" display="Hobo Logger #496" xr:uid="{603BCDBE-C731-8B46-81AE-304776C366B2}"/>
     <hyperlink ref="A3" r:id="rId4" display="Hobo Logger #496" xr:uid="{B5A7B15F-0B57-8E42-9D7D-FD69F32F297F}"/>
-    <hyperlink ref="A15" r:id="rId5" location="/metadata/sagehen_cycles" xr:uid="{3D1FE982-4097-2048-BA2C-BCE8DB50DFEC}"/>
-    <hyperlink ref="A16" r:id="rId6" xr:uid="{59719DCC-3E1F-4B43-B3E1-9D0BFF552A0D}"/>
+    <hyperlink ref="A16" r:id="rId5" location="/metadata/sagehen_cycles" xr:uid="{3D1FE982-4097-2048-BA2C-BCE8DB50DFEC}"/>
+    <hyperlink ref="A17" r:id="rId6" xr:uid="{59719DCC-3E1F-4B43-B3E1-9D0BFF552A0D}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
added Dendra climate download, README
climate data from Water Years 2015-2020 included in the new csv.
</commit_message>
<xml_diff>
--- a/data/station_instrumentation/climate/climate_metadata.xlsx
+++ b/data/station_instrumentation/climate/climate_metadata.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnat/Documents/GitHub/sagehen_meadows/data/station_instrumentation/climate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C72650B-AF1E-D44D-9C4B-A59C33944994}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41310FF-C199-AD43-AACA-8E56059EAA00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="32780" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="3700" windowWidth="29080" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - climate_metadata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
   <si>
     <t>Source</t>
   </si>
@@ -133,9 +144,6 @@
     <t>Wind Speed at 25ft (MS)</t>
   </si>
   <si>
-    <t>Not Found in Dendra: irradiance, solar flux, vapor pressure deficit</t>
-  </si>
-  <si>
     <t>Many Well Locations</t>
   </si>
   <si>
@@ -151,16 +159,40 @@
     <t>The stage recorders were downloaded infrequently and often failed; as a result, data gaps of up to a year in length are found in several of the stage records and up to 2 years in some groundwater wells.</t>
   </si>
   <si>
-    <t>sagehen_metadata.txt has a lot more detailed and helpful information.</t>
-  </si>
-  <si>
-    <t>Scholarworks same location as Dendra? One of the three towers might be Dendra data (Tower 1?)</t>
-  </si>
-  <si>
     <t>Relative Humidity</t>
   </si>
   <si>
     <t xml:space="preserve">Snow Water Equivalent (SWE), </t>
+  </si>
+  <si>
+    <t>at Field Station (East Meadow); use this for East wells and Hobo temp for Kiln?</t>
+  </si>
+  <si>
+    <t>major covariate to consider becuase it drives photosynthesis and transpiaration.</t>
+  </si>
+  <si>
+    <t>less important covariate??</t>
+  </si>
+  <si>
+    <t>precip = snow + rainfall? we want to consider in "realtime" (e.g. to explain a rapid rise in gw) but also lagtime where lagtime = previous water year (e.g. oct-oct to explain differences between years)</t>
+  </si>
+  <si>
+    <t>snow depth does not incorporate snow water equivalent (e.g. some snow might be more water dense than others for the same thickness).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">want to consider in "realtime" but interesting to consider differences between years (e.g. ratio of rain to snow between years). </t>
+  </si>
+  <si>
+    <t>important to evapotranspiration; consider a derived metric of "vapor pressure deficit" (fn of temp + humidity). See Butler paper.</t>
+  </si>
+  <si>
+    <t>role in evaporation, not sure if transpiration?</t>
+  </si>
+  <si>
+    <t>important covariate to consider for differences between years; not reported in Dendra, can we derive?</t>
+  </si>
+  <si>
+    <t>sagehen_metadata.txt has a lot more detailed and helpful information. Scholarworks same location as Dendra? One of the three towers might be Dendra data (Tower 1?)</t>
   </si>
 </sst>
 </file>
@@ -304,7 +336,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -355,6 +387,12 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1517,10 +1555,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>
@@ -1740,7 +1778,9 @@
       <c r="I7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="J7" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="156">
@@ -1771,7 +1811,9 @@
       <c r="I8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="156">
@@ -1802,10 +1844,12 @@
       <c r="I9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="17" t="s">
+        <v>44</v>
+      </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="182">
+    <row r="10" spans="1:11" ht="208">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1833,10 +1877,12 @@
       <c r="I10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="J10" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="78">
+    <row r="11" spans="1:11" ht="156">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1864,8 +1910,11 @@
       <c r="I11" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="J11" s="18" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" ht="25">
+    <row r="12" spans="1:11" ht="156">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -1879,7 +1928,7 @@
         <v>1931.5175999999999</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>26</v>
@@ -1893,8 +1942,11 @@
       <c r="I12" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="J12" s="18" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" ht="25">
+    <row r="13" spans="1:11" ht="130">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1903,10 +1955,13 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="16" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="25">
+    <row r="14" spans="1:11" ht="156">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -1920,7 +1975,7 @@
         <v>1931.5175999999999</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>26</v>
@@ -1932,7 +1987,10 @@
         <v>29</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="104">
@@ -1963,7 +2021,9 @@
       <c r="I15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="5"/>
+      <c r="J15" s="17" t="s">
+        <v>51</v>
+      </c>
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="208">
@@ -1971,7 +2031,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1983,17 +2043,17 @@
         <v>39721.979166666664</v>
       </c>
       <c r="H16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>42</v>
       </c>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" ht="25">
+    <row r="17" spans="1:11" ht="182">
       <c r="A17" s="11" t="s">
         <v>7</v>
       </c>
@@ -2009,8 +2069,8 @@
       <c r="I17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>43</v>
+      <c r="J17" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="K17" s="5"/>
     </row>
@@ -2029,18 +2089,6 @@
     </row>
     <row r="19" spans="1:11" ht="25">
       <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:11" ht="25">
-      <c r="A20" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" ht="20" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
minor updates, new 2021 gw data
</commit_message>
<xml_diff>
--- a/data/station_instrumentation/climate/climate_metadata.xlsx
+++ b/data/station_instrumentation/climate/climate_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnat/Documents/GitHub/sagehen_meadows/data/station_instrumentation/climate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41310FF-C199-AD43-AACA-8E56059EAA00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA39C9B5-ADD1-B144-AEAB-91EA4AF0152B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="3700" windowWidth="29080" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10740" yWindow="980" windowWidth="28600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - climate_metadata" sheetId="1" r:id="rId1"/>
@@ -336,7 +336,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -364,9 +364,6 @@
     <xf numFmtId="22" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -379,20 +376,35 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1557,19 +1569,19 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="81" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="28.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="24.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="50.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44" style="1" bestFit="1" customWidth="1"/>
@@ -1579,17 +1591,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="25">
       <c r="A2" s="2" t="s">
@@ -1601,7 +1613,7 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="18" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1636,7 +1648,7 @@
       <c r="C3" s="4">
         <v>697078.01699999999</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="19">
         <v>1960</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -1667,7 +1679,7 @@
       <c r="C4" s="4">
         <v>697571.46600000001</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="19">
         <v>1939</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -1698,7 +1710,7 @@
       <c r="C5" s="4">
         <v>698064.64199999999</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="19">
         <v>1916</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -1729,7 +1741,7 @@
       <c r="C6" s="4">
         <v>697341.37600000005</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="19">
         <v>1987</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1760,16 +1772,16 @@
       <c r="C7" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="20">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="13">
         <v>43009</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="13">
         <v>43770</v>
       </c>
       <c r="H7" s="5" t="s">
@@ -1778,7 +1790,7 @@
       <c r="I7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="15" t="s">
         <v>45</v>
       </c>
       <c r="K7" s="5"/>
@@ -1793,16 +1805,16 @@
       <c r="C8" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="20">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="13">
         <v>43009</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="13">
         <v>43770</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -1826,10 +1838,10 @@
       <c r="C9" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="20">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
@@ -1844,12 +1856,12 @@
       <c r="I9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="15" t="s">
         <v>44</v>
       </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="208">
+    <row r="10" spans="1:11" ht="234">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1859,10 +1871,10 @@
       <c r="C10" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="20">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F10" s="7" t="s">
@@ -1877,7 +1889,7 @@
       <c r="I10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="15" t="s">
         <v>47</v>
       </c>
       <c r="K10" s="5"/>
@@ -1892,10 +1904,10 @@
       <c r="C11" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="20">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="7" t="s">
@@ -1910,7 +1922,7 @@
       <c r="I11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="J11" s="16" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1924,7 +1936,7 @@
       <c r="C12" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="20">
         <v>1931.5175999999999</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1942,7 +1954,7 @@
       <c r="I12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="16" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1950,14 +1962,14 @@
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="20"/>
       <c r="F13" s="7"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1971,7 +1983,7 @@
       <c r="C14" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="20">
         <v>1931.5175999999999</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1989,7 +2001,7 @@
       <c r="I14" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2003,10 +2015,10 @@
       <c r="C15" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="20">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>35</v>
       </c>
       <c r="F15" s="7" t="s">
@@ -2021,20 +2033,20 @@
       <c r="I15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="15" t="s">
         <v>51</v>
       </c>
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="208">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="5"/>
       <c r="F16" s="8">
         <v>38626</v>
@@ -2048,18 +2060,18 @@
       <c r="I16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="11" t="s">
         <v>41</v>
       </c>
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" ht="182">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="7" t="s">
@@ -2069,16 +2081,16 @@
       <c r="I17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="18" t="s">
+      <c r="J17" s="16" t="s">
         <v>53</v>
       </c>
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" ht="25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="D18" s="21"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="7"/>

</xml_diff>

<commit_message>
Updated climate data and metadata
* PRISM data downloaded directly, included csv for each meadow site (east, kiln, lower, upper) because they offer an interpolated dataset. It's about 2 km between each site.
* Updated climate_metadata with PRISM and GridMET info
</commit_message>
<xml_diff>
--- a/data/station_instrumentation/climate/climate_metadata.xlsx
+++ b/data/station_instrumentation/climate/climate_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnat/Documents/GitHub/sagehen_meadows/data/station_instrumentation/climate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76946C0-0943-E24B-950B-35794522520C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3F78AB-1BD6-C041-844A-73F37D4F2946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15940" yWindow="2000" windowWidth="21960" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10420" yWindow="460" windowWidth="26280" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - climate_metadata" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="80">
   <si>
     <t>Source</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Scholarworks</t>
   </si>
   <si>
-    <t>to 2017</t>
-  </si>
-  <si>
     <t>Sensor</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Campbell Rain Gage TB4-L</t>
   </si>
   <si>
-    <t>GEONOR All Weather Precipitation – Rain Gauge T-200B</t>
-  </si>
-  <si>
     <t>LI-COR PAR sensor LI190SB-L</t>
   </si>
   <si>
@@ -192,10 +186,91 @@
     <t>important covariate to consider for differences between years; not reported in Dendra, can we derive?</t>
   </si>
   <si>
-    <t>sagehen_metadata.txt has a lot more detailed and helpful information. Scholarworks same location as Dendra? One of the three towers might be Dendra data (Tower 1?)</t>
-  </si>
-  <si>
-    <t>ClimateEngine</t>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>Max and Min Vapor Pressure Deficit (kPa)</t>
+  </si>
+  <si>
+    <t>Precipitation (mm)</t>
+  </si>
+  <si>
+    <t>4000 m resolution (covers approx all of Sagehen basin)</t>
+  </si>
+  <si>
+    <t>Max, Min and Mean Temp (C)</t>
+  </si>
+  <si>
+    <t>ClimateEngine / gridMET</t>
+  </si>
+  <si>
+    <t>hourly</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>GEONOR All Weather Precipitation Rain Gauge T-200B</t>
+  </si>
+  <si>
+    <t>Precipitation, Temperature, SWE, Snow Depth</t>
+  </si>
+  <si>
+    <t>Precipitation, Temperature, SWE, Snow Depth, RH, Solar Radiation.</t>
+  </si>
+  <si>
+    <t>from NOAA COOP Station at Sagehen</t>
+  </si>
+  <si>
+    <t>Tower 1 (1934 m)</t>
+  </si>
+  <si>
+    <t>Tower 4 (2350 m)</t>
+  </si>
+  <si>
+    <t>Tower 3 (2114 m)</t>
+  </si>
+  <si>
+    <t>hourly?</t>
+  </si>
+  <si>
+    <t>Precipitation, Temperature, RH, Solar Radiation, Barometric Pressure, SWE, Snow Depth</t>
+  </si>
+  <si>
+    <t>see metadata</t>
+  </si>
+  <si>
+    <t>see PRISM</t>
+  </si>
+  <si>
+    <t>see PRISM; they also offer 30-yr normals (1991-2020) at 800 m resolution.</t>
+  </si>
+  <si>
+    <t>PRISM</t>
+  </si>
+  <si>
+    <t>present</t>
+  </si>
+  <si>
+    <t>every 5 days?</t>
+  </si>
+  <si>
+    <t>4000 m resolution (covers approx all of Sagehen basin); direct download from PRISM gives interpolated results</t>
+  </si>
+  <si>
+    <t>any point</t>
+  </si>
+  <si>
+    <t>see gridMET metadata</t>
+  </si>
+  <si>
+    <t>Precip, VPD, grass ET, Palmer Drought Severity Index (PDSI)</t>
   </si>
 </sst>
 </file>
@@ -339,7 +414,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -358,15 +433,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -376,9 +445,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -405,6 +471,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1567,21 +1663,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34" style="1" customWidth="1"/>
+    <col min="1" max="1" width="39.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="34.83203125" style="17" customWidth="1"/>
     <col min="8" max="8" width="24.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="50.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44" style="1" bestFit="1" customWidth="1"/>
@@ -1591,17 +1687,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="25">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:11" ht="25">
       <c r="A2" s="2" t="s">
@@ -1613,23 +1709,23 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>19</v>
+      <c r="D2" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>3</v>
@@ -1640,7 +1736,7 @@
     </row>
     <row r="3" spans="1:11" ht="25">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4">
         <v>2151456.3659999999</v>
@@ -1648,30 +1744,30 @@
       <c r="C3" s="4">
         <v>697078.01699999999</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="14">
         <v>1960</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="6">
+        <v>17</v>
+      </c>
+      <c r="F3" s="22">
         <v>42696</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="22">
         <v>44099.54960648148</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" ht="25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4">
         <v>2151936.7719999999</v>
@@ -1679,30 +1775,30 @@
       <c r="C4" s="4">
         <v>697571.46600000001</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="14">
         <v>1939</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="8">
+        <v>17</v>
+      </c>
+      <c r="F4" s="23">
         <v>42705</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="22">
         <v>44040.551678240743</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" ht="25">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4">
         <v>2152441.1690000002</v>
@@ -1710,23 +1806,23 @@
       <c r="C5" s="4">
         <v>698064.64199999999</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="14">
         <v>1916</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="8">
+        <v>17</v>
+      </c>
+      <c r="F5" s="23">
         <v>42705</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="23">
         <v>44040.556261574071</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -1741,30 +1837,30 @@
       <c r="C6" s="4">
         <v>697341.37600000005</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="14">
         <v>1987</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="8">
+        <v>17</v>
+      </c>
+      <c r="F6" s="23">
         <v>43239</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="23">
         <v>44056.402777777781</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="104">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5">
         <v>2151773.3686099998</v>
@@ -1772,32 +1868,32 @@
       <c r="C7" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="15">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="24">
+        <v>43009</v>
+      </c>
+      <c r="G7" s="24">
+        <v>43770</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="12">
-        <v>43009</v>
-      </c>
-      <c r="G7" s="12">
-        <v>43770</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>45</v>
+      <c r="J7" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="104">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5">
         <v>2151773.3686099998</v>
@@ -1805,32 +1901,32 @@
       <c r="C8" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="15">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="12">
+      <c r="E8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="24">
         <v>43009</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="24">
         <v>43770</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="104">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5">
         <v>2151773.3686099998</v>
@@ -1838,32 +1934,32 @@
       <c r="C9" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="15">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>44</v>
+      <c r="J9" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" ht="234">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="5">
         <v>2151773.3686099998</v>
@@ -1871,32 +1967,32 @@
       <c r="C10" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="15">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="H10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>47</v>
+      <c r="J10" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" ht="156">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5">
         <v>2151773.3686099998</v>
@@ -1904,31 +2000,31 @@
       <c r="C11" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="15">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="H11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>49</v>
+        <v>28</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="156">
       <c r="A12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5">
         <v>2151773.3686099998</v>
@@ -1936,46 +2032,46 @@
       <c r="C12" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="15">
         <v>1931.5175999999999</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="H12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>48</v>
+        <v>28</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="130">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="18"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="5"/>
+      <c r="D13" s="15"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>52</v>
+      <c r="I13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="156">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="5">
         <v>2151773.3686099998</v>
@@ -1983,31 +2079,31 @@
       <c r="C14" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="15">
         <v>1931.5175999999999</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="H14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>50</v>
+        <v>28</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="78">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="5">
         <v>2151773.3686099998</v>
@@ -2015,94 +2111,297 @@
       <c r="C15" s="5">
         <v>697491.42197100003</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="15">
         <v>1931.5175999999999</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="234">
+      <c r="A16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" s="7" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="16"/>
+      <c r="F16" s="23">
+        <v>38626</v>
+      </c>
+      <c r="G16" s="23">
+        <v>39721.979166666664</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" ht="234">
-      <c r="A16" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="8">
-        <v>38626</v>
-      </c>
-      <c r="G16" s="8">
-        <v>39721.979166666664</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>41</v>
+      <c r="J16" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" ht="182">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:11" ht="52">
+      <c r="A17" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>53</v>
+      <c r="D17" s="16"/>
+      <c r="E17" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="16">
+        <v>1953</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11" ht="25">
-      <c r="A18" s="10" t="s">
-        <v>54</v>
+    <row r="18" spans="1:11" ht="78">
+      <c r="A18" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="7"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="16">
+        <v>2001</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:11" ht="25">
-      <c r="I19" s="7"/>
+    <row r="19" spans="1:11" ht="104">
+      <c r="A19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="16">
+        <v>2009</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" ht="104">
+      <c r="A20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="16">
+        <v>2009</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="104">
+      <c r="A21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="16">
+        <v>2009</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J21" s="12"/>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" ht="128" customHeight="1">
+      <c r="A22" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="16">
+        <v>1981</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" ht="114" customHeight="1">
+      <c r="A23" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1981</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="102" customHeight="1">
+      <c r="A24" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="16">
+        <v>1981</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="91" customHeight="1">
+      <c r="A25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="20" customHeight="1">
+      <c r="I27" s="5"/>
+      <c r="J27" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2115,7 +2414,20 @@
     <hyperlink ref="A3" r:id="rId4" display="Hobo Logger #496" xr:uid="{B5A7B15F-0B57-8E42-9D7D-FD69F32F297F}"/>
     <hyperlink ref="A16" r:id="rId5" location="/metadata/sagehen_cycles" xr:uid="{3D1FE982-4097-2048-BA2C-BCE8DB50DFEC}"/>
     <hyperlink ref="A17" r:id="rId6" xr:uid="{59719DCC-3E1F-4B43-B3E1-9D0BFF552A0D}"/>
-    <hyperlink ref="A18" r:id="rId7" xr:uid="{EE7E7994-1EC2-A546-93A0-681753C51BA7}"/>
+    <hyperlink ref="A22" r:id="rId7" xr:uid="{EE7E7994-1EC2-A546-93A0-681753C51BA7}"/>
+    <hyperlink ref="A25" r:id="rId8" display="ClimateEngine" xr:uid="{449B054D-99AF-B848-A848-ACD40B5932B0}"/>
+    <hyperlink ref="A18" r:id="rId9" xr:uid="{56BBF8DA-8627-5641-B315-2DFDCC8A6B05}"/>
+    <hyperlink ref="A19" r:id="rId10" xr:uid="{54CD2AAF-0A63-8448-AFB3-B38F7826F261}"/>
+    <hyperlink ref="A20" r:id="rId11" xr:uid="{21CECC94-6172-1340-B8DD-8A9C6AABC7AA}"/>
+    <hyperlink ref="A21" r:id="rId12" xr:uid="{31C2A64E-8AC5-4A40-92A5-797A46A85082}"/>
+    <hyperlink ref="E17" r:id="rId13" xr:uid="{B71DFA68-A155-EA45-AEA0-32CBD0CCA7B1}"/>
+    <hyperlink ref="E18:E21" r:id="rId14" display="see metadata" xr:uid="{A234D4B8-73E3-4142-B000-85754BBB4D3B}"/>
+    <hyperlink ref="E22" r:id="rId15" display="see PRISM" xr:uid="{9AA09AB9-ECDB-2C4E-950D-1F999C269F07}"/>
+    <hyperlink ref="E23" r:id="rId16" xr:uid="{4B0BBF5B-2117-9D42-A860-23710A7BA32B}"/>
+    <hyperlink ref="E24" r:id="rId17" xr:uid="{270B6EDE-B195-6C48-9E1C-28C8F7EBA145}"/>
+    <hyperlink ref="A23" r:id="rId18" xr:uid="{A924FE56-C677-4D4C-A9A7-D623CC08495E}"/>
+    <hyperlink ref="A24" r:id="rId19" xr:uid="{996C0FF3-242F-D441-B026-E173C2041167}"/>
+    <hyperlink ref="E25" r:id="rId20" xr:uid="{1A5BE9A5-3C75-6D49-BC9E-C1BEAA14C12D}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
climate data processing scripts
Includes quick jupyter notebook scripts to check completeness of Dendra data.
Large file from Dendra not committed due to size, not allowed; still processing the data.
</commit_message>
<xml_diff>
--- a/data/station_instrumentation/climate/climate_metadata.xlsx
+++ b/data/station_instrumentation/climate/climate_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SANDISK_SSD_G40/GoogleDrive/GitHub/sagehen_meadows/data/station_instrumentation/climate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8C8462-FE80-C343-90C5-5941239AB29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6299815-0AE9-DE41-BAEB-1F71DB1C6E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="1620" windowWidth="36420" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,9 +138,6 @@
     <t>Wind Speed at 25ft (MS)</t>
   </si>
   <si>
-    <t>Many Well Locations</t>
-  </si>
-  <si>
     <t>Groundwater Level (mm)</t>
   </si>
   <si>
@@ -159,12 +156,6 @@
     <t>at Field Station (East Meadow); use this for East wells and Hobo temp for Kiln?</t>
   </si>
   <si>
-    <t>major covariate to consider becuase it drives photosynthesis and transpiaration.</t>
-  </si>
-  <si>
-    <t>less important covariate??</t>
-  </si>
-  <si>
     <t>precip = snow + rainfall? we want to consider in "realtime" (e.g. to explain a rapid rise in gw) but also lagtime where lagtime = previous water year (e.g. oct-oct to explain differences between years)</t>
   </si>
   <si>
@@ -316,6 +307,15 @@
   </si>
   <si>
     <t>temperature, precipiation quantity, snowfall, and snowpack characteristics including 24-hour snowfall, snowpack depth, and snow water equivalent for each water year (October 1 to September 30) from 1971 to 2019</t>
+  </si>
+  <si>
+    <t>major covariate to consider because it drives photosynthesis and transpiaration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">potential covariate for groundwater levels </t>
+  </si>
+  <si>
+    <t>Many Well Locations at Sagehen East and Kiln Meadows</t>
   </si>
 </sst>
 </file>
@@ -552,15 +552,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -571,6 +568,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1736,8 +1736,8 @@
   </sheetPr>
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>
@@ -1756,7 +1756,7 @@
     <col min="13" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="32" customFormat="1" ht="34">
+    <row r="1" spans="1:11" s="21" customFormat="1" ht="34">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K2" s="9"/>
     </row>
@@ -1853,7 +1853,7 @@
         <v>20</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K3" s="9"/>
     </row>
@@ -1886,7 +1886,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K4" s="9"/>
     </row>
@@ -1919,13 +1919,13 @@
         <v>20</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" ht="17">
+    <row r="6" spans="1:11" s="5" customFormat="1" ht="34">
       <c r="A6" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="7"/>
@@ -1936,13 +1936,13 @@
       <c r="H6" s="9"/>
       <c r="I6" s="11"/>
       <c r="J6" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="17">
       <c r="A7" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="7"/>
@@ -1953,13 +1953,13 @@
       <c r="H7" s="9"/>
       <c r="I7" s="11"/>
       <c r="J7" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" ht="89" customHeight="1">
-      <c r="A8" s="34" t="s">
-        <v>86</v>
+      <c r="A8" s="33" t="s">
+        <v>83</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="7"/>
@@ -1968,21 +1968,21 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="36" t="s">
-        <v>94</v>
+      <c r="I8" s="35" t="s">
+        <v>91</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="34">
-      <c r="A9" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>89</v>
+      <c r="A9" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>86</v>
       </c>
       <c r="D9" s="8">
         <v>2127.5039999999999</v>
@@ -1995,23 +1995,23 @@
         <v>26</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>90</v>
+        <v>55</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>87</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" ht="34">
-      <c r="A10" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>93</v>
+      <c r="A10" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>90</v>
       </c>
       <c r="D10" s="8">
         <v>2541.422</v>
@@ -2024,10 +2024,10 @@
         <v>26</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="33" t="s">
-        <v>90</v>
+        <v>55</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>87</v>
       </c>
       <c r="J10" s="21"/>
       <c r="K10" s="9"/>
@@ -2061,7 +2061,7 @@
         <v>23</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="K11" s="9"/>
     </row>
@@ -2094,7 +2094,7 @@
         <v>24</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="K12" s="9"/>
     </row>
@@ -2127,7 +2127,7 @@
         <v>27</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K13" s="9"/>
     </row>
@@ -2145,7 +2145,7 @@
         <v>1931.5175999999999</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>25</v>
@@ -2160,7 +2160,7 @@
         <v>29</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K14" s="9"/>
     </row>
@@ -2193,7 +2193,7 @@
         <v>30</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="5" customFormat="1" ht="68">
@@ -2210,7 +2210,7 @@
         <v>1931.5175999999999</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>25</v>
@@ -2225,7 +2225,7 @@
         <v>31</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="5" customFormat="1" ht="51">
@@ -2242,7 +2242,7 @@
         <v>1931.5175999999999</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>25</v>
@@ -2254,10 +2254,10 @@
         <v>28</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J17" s="21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="5" customFormat="1" ht="17">
@@ -2289,7 +2289,7 @@
         <v>34</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K18" s="9"/>
     </row>
@@ -2297,8 +2297,8 @@
       <c r="A19" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>35</v>
+      <c r="B19" s="36" t="s">
+        <v>94</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="20"/>
@@ -2309,17 +2309,17 @@
         <v>39721.979166666664</v>
       </c>
       <c r="H19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J19" s="22" t="s">
-        <v>39</v>
-      </c>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" s="5" customFormat="1" ht="17">
+    <row r="20" spans="1:11" s="5" customFormat="1" ht="34">
       <c r="A20" s="14" t="s">
         <v>7</v>
       </c>
@@ -2327,22 +2327,22 @@
       <c r="C20" s="9"/>
       <c r="D20" s="20"/>
       <c r="E20" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F20" s="20">
         <v>1953</v>
       </c>
       <c r="G20" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H20" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>60</v>
-      </c>
       <c r="J20" s="21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K20" s="9"/>
     </row>
@@ -2354,211 +2354,211 @@
       <c r="C21" s="9"/>
       <c r="D21" s="25"/>
       <c r="E21" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F21" s="20">
         <v>2001</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I21" s="21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J21" s="21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="1:11" s="5" customFormat="1" ht="34">
+    <row r="22" spans="1:11" s="5" customFormat="1" ht="51">
       <c r="A22" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="25"/>
       <c r="E22" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F22" s="20">
         <v>2009</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="1:11" s="5" customFormat="1" ht="34">
+    <row r="23" spans="1:11" s="5" customFormat="1" ht="51">
       <c r="A23" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="25"/>
       <c r="E23" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F23" s="20">
         <v>2009</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I23" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J23" s="21"/>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="1:11" s="5" customFormat="1" ht="34">
+    <row r="24" spans="1:11" s="5" customFormat="1" ht="51">
       <c r="A24" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="25"/>
       <c r="E24" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F24" s="20">
         <v>2009</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J24" s="21"/>
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:11" s="5" customFormat="1" ht="128" customHeight="1">
       <c r="A25" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="15"/>
       <c r="E25" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F25" s="20">
         <v>1981</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" s="5" customFormat="1" ht="114" customHeight="1">
       <c r="A26" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="15"/>
       <c r="E26" s="23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F26" s="20">
         <v>1981</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J26" s="27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="5" customFormat="1" ht="102" customHeight="1">
       <c r="A27" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="15"/>
       <c r="E27" s="23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F27" s="20">
         <v>1981</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="5" customFormat="1" ht="91" customHeight="1">
       <c r="A28" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D28" s="28"/>
       <c r="E28" s="29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
       <c r="H28" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J28" s="21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="20" customHeight="1">

</xml_diff>